<commit_message>
Touched up sample form.
</commit_message>
<xml_diff>
--- a/extras/sample-form/Decryption field plug-in sample form.xlsx
+++ b/extras/sample-form/Decryption field plug-in sample form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/decrypt/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E81DA4-0B6D-524A-9D72-1DC9CE01F63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA313927-F99C-CB41-B439-35D6E7072A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28780" yWindow="500" windowWidth="28800" windowHeight="16640" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="400">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2488,9 +2488,6 @@
     <t>key</t>
   </si>
   <si>
-    <t>ciphertext</t>
-  </si>
-  <si>
     <t>decrypt</t>
   </si>
   <si>
@@ -2506,18 +2503,12 @@
     <t>Manual entry</t>
   </si>
   <si>
-    <t>How would you like to enter the information?</t>
-  </si>
-  <si>
     <t>enter_key</t>
   </si>
   <si>
     <t>Enter the decryption key:</t>
   </si>
   <si>
-    <t>'S+iTPOq1mSx4PQrcLyTcqA=='</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -2558,9 +2549,6 @@
   </si>
   <si>
     <t>item-at('|', ${decrypt}, 1)</t>
-  </si>
-  <si>
-    <t>Decrypted data:</t>
   </si>
   <si>
     <t>disp</t>
@@ -2609,6 +2597,12 @@
 0=${enc_resp_name},
 1=${enc_age},
 2=${enc_marital})</t>
+  </si>
+  <si>
+    <t>Decryption results:</t>
+  </si>
+  <si>
+    <t>How would you like to enter the decryption key?</t>
   </si>
 </sst>
 </file>
@@ -3173,7 +3167,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3349,7 +3343,6 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3527,6 +3520,64 @@
   <dxfs count="123">
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
@@ -3536,6 +3587,50 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFEEB400"/>
         </patternFill>
       </fill>
@@ -3578,6 +3673,39 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="6" tint="0.59999389629810485"/>
@@ -3586,8 +3714,9 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3602,6 +3731,21 @@
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3615,6 +3759,350 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFBFB00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFDCC97A"/>
@@ -3623,96 +4111,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFE4E300"/>
@@ -3721,54 +4119,15 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFEEB400"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor rgb="FFEEB400"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3776,372 +4135,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFBFB00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4193,7 +4186,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEAEB74"/>
+          <bgColor rgb="FFE3E0CF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4201,6 +4194,14 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4214,16 +4215,8 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
+          <bgColor rgb="FFEAEB74"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4283,6 +4276,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -4295,7 +4295,73 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF6969"/>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4309,14 +4375,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4332,23 +4391,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4362,22 +4405,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4390,13 +4418,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -4408,13 +4429,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -4427,21 +4441,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4449,13 +4449,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFBBBB59"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4874,13 +4867,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W27"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5071,18 +5064,18 @@
     </row>
     <row r="11" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>370</v>
+        <v>399</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="9" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5090,16 +5083,16 @@
         <v>87</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5107,19 +5100,19 @@
         <v>68</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="K13" s="9" t="s">
         <v>371</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>395</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -5130,7 +5123,7 @@
         <v>363</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5138,13 +5131,13 @@
         <v>68</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -5152,10 +5145,10 @@
         <v>120</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -5163,10 +5156,10 @@
         <v>120</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -5174,35 +5167,38 @@
         <v>120</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="N21" s="71" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="C21" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>365</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>388</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>401</v>
+        <v>381</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -5210,10 +5206,10 @@
         <v>120</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="N23" s="9" t="s">
         <v>384</v>
-      </c>
-      <c r="N23" s="9" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -5221,108 +5217,97 @@
         <v>120</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>399</v>
+        <v>382</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B25" s="9" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="N25" s="9" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="136" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>389</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>398</v>
+      <c r="C26" s="10" t="s">
+        <v>394</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:W1048576">
-    <cfRule type="expression" dxfId="122" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="2" stopIfTrue="1">
+      <formula>$A1="file"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="121" priority="6" stopIfTrue="1">
+      <formula>$A1="enumerator"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="120" priority="10" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="119" priority="13" stopIfTrue="1">
+      <formula>$A1="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="17" stopIfTrue="1">
+      <formula>OR($A1="audio", $A1="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="117" priority="19" stopIfTrue="1">
+      <formula>$A1="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="23" stopIfTrue="1">
+      <formula>OR($A1="date", $A1="datetime", $A1="time")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="25" stopIfTrue="1">
+      <formula>OR($A1="calculate", $A1="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="114" priority="27" stopIfTrue="1">
+      <formula>$A1="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="113" priority="29" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="2" stopIfTrue="1">
-      <formula>$A1="file"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="120" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="31" stopIfTrue="1">
+      <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="111" priority="33" stopIfTrue="1">
+      <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="36" stopIfTrue="1">
+      <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="43" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="48" stopIfTrue="1">
+      <formula>$A1="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="107" priority="50" stopIfTrue="1">
+      <formula>$A1="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="52" stopIfTrue="1">
+      <formula>$A1="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="53" stopIfTrue="1">
+      <formula>$A1="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="55" stopIfTrue="1">
+      <formula>$A1="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="56" stopIfTrue="1">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="6" stopIfTrue="1">
-      <formula>$A1="enumerator"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="118" priority="55" stopIfTrue="1">
-      <formula>$A1="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="117" priority="10" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="116" priority="53" stopIfTrue="1">
-      <formula>$A1="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="115" priority="13" stopIfTrue="1">
-      <formula>$A1="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="114" priority="52" stopIfTrue="1">
-      <formula>$A1="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="113" priority="17" stopIfTrue="1">
-      <formula>OR($A1="audio", $A1="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="112" priority="50" stopIfTrue="1">
-      <formula>$A1="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="111" priority="19" stopIfTrue="1">
-      <formula>$A1="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="48" stopIfTrue="1">
-      <formula>$A1="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="109" priority="23" stopIfTrue="1">
-      <formula>OR($A1="date", $A1="datetime", $A1="time")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="108" priority="43" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="107" priority="25" stopIfTrue="1">
-      <formula>OR($A1="calculate", $A1="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="36" stopIfTrue="1">
-      <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="27" stopIfTrue="1">
-      <formula>$A1="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="104" priority="33" stopIfTrue="1">
-      <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="58" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="31" stopIfTrue="1">
-      <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="101" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="9" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="32" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="100" priority="9" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576 N1:N1048576">
@@ -5357,20 +5342,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="92" priority="30" stopIfTrue="1">
-      <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="91" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="1" stopIfTrue="1">
+      <formula>$A1="file"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="16" stopIfTrue="1">
+      <formula>OR($A1="audio", $A1="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="90" priority="26" stopIfTrue="1">
       <formula>$A1="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="90" priority="16" stopIfTrue="1">
-      <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="89" priority="28" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="1" stopIfTrue="1">
-      <formula>$A1="file"</formula>
+    <cfRule type="expression" dxfId="88" priority="30" stopIfTrue="1">
+      <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1048576 F1:F1048576">
@@ -5454,24 +5439,24 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B4" s="15">
         <v>1</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B5" s="15">
         <v>2</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -5559,14 +5544,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C2" s="16" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2403192031</v>
+        <v>2403201333</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>362</v>
@@ -5601,26 +5586,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="76"/>
+      <c r="B1" s="75"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A2" s="77"/>
-      <c r="B2" s="78"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="77"/>
     </row>
     <row r="3" spans="1:30" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="78" t="s">
         <v>299</v>
       </c>
-      <c r="B3" s="80"/>
+      <c r="B3" s="79"/>
     </row>
     <row r="4" spans="1:30" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="82" t="s">
         <v>325</v>
       </c>
-      <c r="B4" s="84"/>
+      <c r="B4" s="83"/>
     </row>
     <row r="6" spans="1:30" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="53" t="s">
@@ -5885,10 +5870,10 @@
       </c>
     </row>
     <row r="10" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="80" t="s">
         <v>224</v>
       </c>
-      <c r="B10" s="81"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -8911,19 +8896,19 @@
       <c r="AD89" s="32"/>
     </row>
     <row r="91" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A91" s="82" t="s">
+      <c r="A91" s="81" t="s">
         <v>291</v>
       </c>
-      <c r="B91" s="82"/>
+      <c r="B91" s="81"/>
       <c r="C91" s="42"/>
       <c r="D91" s="43"/>
     </row>
     <row r="92" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A92" s="72" t="s">
+      <c r="A92" s="71" t="s">
         <v>353</v>
       </c>
-      <c r="B92" s="73"/>
-      <c r="C92" s="74"/>
+      <c r="B92" s="72"/>
+      <c r="C92" s="73"/>
       <c r="D92" s="43"/>
     </row>
     <row r="94" spans="1:30" x14ac:dyDescent="0.2">
@@ -9548,14 +9533,14 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:J6 L6:O6 Q6:S6">
-    <cfRule type="expression" dxfId="82" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="95" stopIfTrue="1">
+      <formula>$A6="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="96" stopIfTrue="1">
+      <formula>$A6="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="80" priority="98" stopIfTrue="1">
       <formula>$A6="begin group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="95" stopIfTrue="1">
-      <formula>$A6="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="80" priority="96" stopIfTrue="1">
-      <formula>$A6="end group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:J6 Q6:S6">
@@ -9586,25 +9571,25 @@
     <cfRule type="expression" dxfId="71" priority="90" stopIfTrue="1">
       <formula>$A6="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
+      <formula>$A6="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
       <formula>$A6="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="69" priority="92" stopIfTrue="1">
-      <formula>$A6="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:J6">
-    <cfRule type="expression" dxfId="68" priority="73" stopIfTrue="1">
-      <formula>OR($A6="date", $A6="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="67" stopIfTrue="1">
       <formula>$A6="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="69" stopIfTrue="1">
+      <formula>OR($A6="audio", $A6="video")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="66" priority="71" stopIfTrue="1">
       <formula>$A6="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="69" stopIfTrue="1">
-      <formula>OR($A6="audio", $A6="video")</formula>
+    <cfRule type="expression" dxfId="65" priority="73" stopIfTrue="1">
+      <formula>OR($A6="date", $A6="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 H6">
@@ -9628,14 +9613,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6 H6">
-    <cfRule type="expression" dxfId="60" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="70" stopIfTrue="1">
+      <formula>$A6="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="72" stopIfTrue="1">
+      <formula>OR($A6="date", $A6="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="85" stopIfTrue="1">
       <formula>OR(AND(LEFT($A6, 16)="select_multiple ", LEN($A6)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A6, 17)))), AND(LEFT($A6, 11)="select_one ", LEN($A6)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A6, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="70" stopIfTrue="1">
-      <formula>$A6="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="72" stopIfTrue="1">
-      <formula>OR($A6="date", $A6="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6 S6 L6">
@@ -9644,14 +9629,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="expression" dxfId="56" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="68" stopIfTrue="1">
+      <formula>OR($A6="audio", $A6="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="76" stopIfTrue="1">
+      <formula>$A6="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="78" stopIfTrue="1">
       <formula>$A6="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="55" priority="68" stopIfTrue="1">
-      <formula>OR($A6="audio", $A6="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="76" stopIfTrue="1">
-      <formula>$A6="note"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="53" priority="80" stopIfTrue="1">
       <formula>$A6="geopoint"</formula>
@@ -9671,86 +9656,86 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="49" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="39" stopIfTrue="1">
+      <formula>OR($A6="audio", $A6="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="40" stopIfTrue="1">
+      <formula>$A6="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="41" stopIfTrue="1">
+      <formula>OR($A6="date", $A6="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="42" stopIfTrue="1">
+      <formula>$A6="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="43" stopIfTrue="1">
+      <formula>$A6="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="44" stopIfTrue="1">
+      <formula>$A6="geopoint"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="45" stopIfTrue="1">
       <formula>OR(AND(LEFT($A6, 16)="select_multiple ", LEN($A6)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A6, 17)))), AND(LEFT($A6, 11)="select_one ", LEN($A6)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A6, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="46" stopIfTrue="1">
       <formula>$A6="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="47" stopIfTrue="1">
       <formula>$A6="begin group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="43" stopIfTrue="1">
-      <formula>$A6="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="44" stopIfTrue="1">
-      <formula>$A6="geopoint"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="42" stopIfTrue="1">
-      <formula>$A6="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="41" stopIfTrue="1">
-      <formula>OR($A6="date", $A6="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="39" stopIfTrue="1">
-      <formula>OR($A6="audio", $A6="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="40" stopIfTrue="1">
-      <formula>$A6="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="40" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="30" stopIfTrue="1">
+      <formula>$A6="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="32" stopIfTrue="1">
+      <formula>$A6="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="36" stopIfTrue="1">
+      <formula>$A6="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="37" stopIfTrue="1">
+      <formula>$A6="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="38" stopIfTrue="1">
       <formula>$A6="begin group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="37" stopIfTrue="1">
-      <formula>$A6="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="30" stopIfTrue="1">
-      <formula>$A6="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="36" stopIfTrue="1">
-      <formula>$A6="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="32" stopIfTrue="1">
-      <formula>$A6="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:O6">
-    <cfRule type="expression" dxfId="35" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="31" stopIfTrue="1">
+      <formula>$A6="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="33" stopIfTrue="1">
+      <formula>$A6="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="34" stopIfTrue="1">
       <formula>$A6="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="31" stopIfTrue="1">
-      <formula>$A6="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="35" stopIfTrue="1">
       <formula>$A6="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="33" stopIfTrue="1">
-      <formula>$A6="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:P6">
-    <cfRule type="expression" dxfId="31" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="5" stopIfTrue="1">
+      <formula>OR($A6="calculate", $A6="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="6" stopIfTrue="1">
+      <formula>$A6="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="7" stopIfTrue="1">
+      <formula>$A6="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="8" stopIfTrue="1">
       <formula>$A6="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="7" stopIfTrue="1">
-      <formula>$A6="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
       <formula>OR($A6="audio audit", $A6="text audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="6" stopIfTrue="1">
-      <formula>$A6="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="11" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A6, 16)="select_multiple ", LEN($A6)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A6, 17)))), AND(LEFT($A6, 11)="select_one ", LEN($A6)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A6, 12)))))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="26" priority="10" stopIfTrue="1">
       <formula>OR($A6="phonenumber", $A6="start", $A6="end", $A6="deviceid", $A6="subscriberid", $A6="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="5" stopIfTrue="1">
-      <formula>OR($A6="calculate", $A6="calculate_here")</formula>
+    <cfRule type="expression" dxfId="25" priority="11" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A6, 16)="select_multiple ", LEN($A6)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A6, 17)))), AND(LEFT($A6, 11)="select_one ", LEN($A6)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A6, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:AD6">
@@ -9791,14 +9776,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T6:AD6">
-    <cfRule type="expression" dxfId="13" priority="54" stopIfTrue="1">
-      <formula>$A6="barcode"</formula>
+    <cfRule type="expression" dxfId="13" priority="52" stopIfTrue="1">
+      <formula>OR($A6="calculate", $A6="calculate_here")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="12" priority="53" stopIfTrue="1">
       <formula>$A6="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="52" stopIfTrue="1">
-      <formula>OR($A6="calculate", $A6="calculate_here")</formula>
+    <cfRule type="expression" dxfId="11" priority="54" stopIfTrue="1">
+      <formula>$A6="barcode"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="55" stopIfTrue="1">
       <formula>$A6="geopoint"</formula>
@@ -9806,8 +9791,8 @@
     <cfRule type="expression" dxfId="9" priority="56" stopIfTrue="1">
       <formula>OR($A6="audio audit", $A6="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="65" stopIfTrue="1">
-      <formula>$A6="begin group"</formula>
+    <cfRule type="expression" dxfId="8" priority="57" stopIfTrue="1">
+      <formula>OR($A6="phonenumber", $A6="start", $A6="end", $A6="deviceid", $A6="subscriberid", $A6="simserial")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="7" priority="58" stopIfTrue="1">
       <formula>OR(AND(LEFT($A6, 16)="select_multiple ", LEN($A6)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A6, 17)))), AND(LEFT($A6, 11)="select_one ", LEN($A6)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A6, 12)))))</formula>
@@ -9830,8 +9815,8 @@
     <cfRule type="expression" dxfId="1" priority="64" stopIfTrue="1">
       <formula>$A6="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="57" stopIfTrue="1">
-      <formula>OR($A6="phonenumber", $A6="start", $A6="end", $A6="deviceid", $A6="subscriberid", $A6="simserial")</formula>
+    <cfRule type="expression" dxfId="0" priority="65" stopIfTrue="1">
+      <formula>$A6="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -9917,38 +9902,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="76"/>
+      <c r="B1" s="75"/>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="44"/>
       <c r="B2" s="45"/>
     </row>
     <row r="3" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="78" t="s">
         <v>302</v>
       </c>
-      <c r="B3" s="80"/>
+      <c r="B3" s="79"/>
     </row>
     <row r="4" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="84" t="s">
         <v>322</v>
       </c>
-      <c r="B4" s="86"/>
+      <c r="B4" s="85"/>
     </row>
     <row r="5" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="B5" s="86"/>
+      <c r="B5" s="85"/>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="82" t="s">
         <v>324</v>
       </c>
-      <c r="B6" s="84"/>
+      <c r="B6" s="83"/>
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
@@ -10043,28 +10028,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="90"/>
+      <c r="B1" s="89"/>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
       <c r="E1" s="36"/>
       <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="91"/>
-      <c r="B2" s="92"/>
+      <c r="A2" s="90"/>
+      <c r="B2" s="91"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
       <c r="E2" s="36"/>
       <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="86" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="88"/>
+      <c r="B3" s="87"/>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
       <c r="E3" s="36"/>

</xml_diff>